<commit_message>
z tests and instructions for notebooks
</commit_message>
<xml_diff>
--- a/assets/df_merge_bls_l1_pivoted.xlsx
+++ b/assets/df_merge_bls_l1_pivoted.xlsx
@@ -5,23 +5,24 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kolbesussman/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kolbesussman/Desktop/SIADS 593/githubrepo/Project/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DFC73B-3CE6-804A-B4D4-D9DEAA3B6EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9E8D12-70A9-B243-AD72-3B141C445FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20920" yWindow="500" windowWidth="23880" windowHeight="22920" xr2:uid="{6B4464F9-13CB-4B27-8BC1-1F1B7F4C824B}"/>
+    <workbookView xWindow="20640" yWindow="500" windowWidth="24160" windowHeight="22920" xr2:uid="{6B4464F9-13CB-4B27-8BC1-1F1B7F4C824B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="df_merge_bls_l1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">df_merge_bls_l1!$A$1:$L$111</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$72:$C$95</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId3"/>
+    <pivotCache cacheId="16" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -528,7 +529,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -763,6 +764,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -809,20 +888,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" pivotButton="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -834,7 +911,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -847,6 +923,31 @@
     <xf numFmtId="0" fontId="17" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" pivotButton="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" pivotButton="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -893,7 +994,7 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="24">
     <dxf>
       <border>
         <left style="medium">
@@ -1183,14 +1284,100 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2879,7 +3066,137 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B92ABA71-3162-AE49-98C4-54AE33BFA5C6}" name="PivotTable5" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E5A9BBA-BED9-49E4-B5B0-821E7F7BD2F3}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A4:C8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="12">
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="23">
+        <item x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item h="1" x="12"/>
+        <item h="1" x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item h="1" x="16"/>
+        <item h="1" x="17"/>
+        <item h="1" x="18"/>
+        <item h="1" x="19"/>
+        <item h="1" x="20"/>
+        <item h="1" x="21"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Sum of number_of_workers_men_sum" fld="8" baseField="0" baseItem="0"/>
+    <dataField name="Sum of number_of_workers_women_sum" fld="10" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="11">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="10">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="9">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B92ABA71-3162-AE49-98C4-54AE33BFA5C6}" name="PivotTable5" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A24:C47" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -3074,26 +3391,26 @@
     <dataField name="Sum of number_of_workers_all_sum" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="5">
+    <format dxfId="17">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="16">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="15">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -3116,8 +3433,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5C1AB623-C2A8-3D4C-BDD6-2F315D160A6A}" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5C1AB623-C2A8-3D4C-BDD6-2F315D160A6A}" name="PivotTable4" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A14:C18" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -3204,156 +3521,26 @@
     <dataField name="Sum of number_of_students_women_sum" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="11">
+    <format dxfId="23">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="22">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="21">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="2">
-            <x v="0"/>
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E5A9BBA-BED9-49E4-B5B0-821E7F7BD2F3}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A4:C8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="12">
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="23">
-        <item x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item h="1" x="4"/>
-        <item h="1" x="5"/>
-        <item h="1" x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item h="1" x="12"/>
-        <item h="1" x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item h="1" x="16"/>
-        <item h="1" x="17"/>
-        <item h="1" x="18"/>
-        <item h="1" x="19"/>
-        <item h="1" x="20"/>
-        <item h="1" x="21"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="0" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Sum of number_of_workers_men_sum" fld="8" baseField="0" baseItem="0"/>
-    <dataField name="Sum of number_of_workers_women_sum" fld="10" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="17">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="16">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="15">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="14">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="13">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="12">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -3695,8 +3882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CB5CF8-83EF-49C2-B5C0-FA9DDEAF8D56}">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3713,305 +3900,282 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
         <v>2015</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="10"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" t="s">
         <v>39</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5">
         <v>2273</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5">
         <v>382</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5">
         <f>C5+B5</f>
         <v>2655</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="13">
         <f>C5/D5</f>
         <v>0.14387947269303203</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6">
         <v>662</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6">
         <v>516</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6">
         <f t="shared" ref="D6:D8" si="0">C6+B6</f>
         <v>1178</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="13">
         <f>C6/D6</f>
         <v>0.43803056027164688</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7">
         <v>7329</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7">
         <v>5146</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>12475</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="13">
         <f>C7/D7</f>
         <v>0.41250501002004009</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8">
         <v>10264</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8">
         <v>6044</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>16308</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="14">
         <f>C8/D8</f>
         <v>0.37061564876134412</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="23"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="9">
+      <c r="A12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="8">
         <v>2015</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
+      <c r="A13" s="10"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15">
         <v>550</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15">
         <v>211</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15">
         <f>C15+B15</f>
         <v>761</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="13">
         <f>C15/D15</f>
         <v>0.27726675427069647</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16">
         <v>964</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16">
         <v>1366</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16">
         <f t="shared" ref="D16:D18" si="1">C16+B16</f>
         <v>2330</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="13">
         <f>C16/D16</f>
         <v>0.58626609442060085</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17">
         <v>27</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17">
         <v>31</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="13">
         <f>C17/D17</f>
         <v>0.53448275862068961</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18">
         <v>1541</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18">
         <v>1608</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
         <v>3149</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="14">
         <f>C18/D18</f>
         <v>0.51063829787234039</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
-    </row>
-    <row r="20" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="24" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="26"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="9">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="23"/>
+    </row>
+    <row r="22" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="25">
         <v>2015</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="38" t="s">
         <v>41</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -4020,546 +4184,546 @@
       <c r="E24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="28">
         <v>761</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="29">
         <v>2655</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="19">
         <f>B25/B$47</f>
         <v>0.15051424050632911</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="19">
         <f>C25/C$47</f>
         <v>2.4339264596683261E-2</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="20">
         <f>E25-D25</f>
         <v>-0.12617497590964585</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="30">
         <v>351</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="26">
         <v>1643</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="19">
         <f t="shared" ref="D26:E47" si="2">B26/B$47</f>
         <v>6.9422468354430375E-2</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="19">
         <f t="shared" si="2"/>
         <v>1.5061925322919245E-2</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="20">
         <f t="shared" ref="F26:F34" si="3">E26-D26</f>
         <v>-5.4360543031511131E-2</v>
       </c>
     </row>
     <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="20">
-        <v>0</v>
-      </c>
-      <c r="C27" s="20">
+      <c r="B27" s="30">
+        <v>0</v>
+      </c>
+      <c r="C27" s="26">
         <v>3603</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="19">
         <f t="shared" si="2"/>
         <v>3.3029894667363384E-2</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="20">
         <f t="shared" si="3"/>
         <v>3.3029894667363384E-2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="20">
+      <c r="B28" s="30">
         <v>40</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="26">
         <v>5943</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="19">
         <f t="shared" si="2"/>
         <v>7.9113924050632917E-3</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="19">
         <f t="shared" si="2"/>
         <v>5.4481449905118121E-2</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="20">
         <f t="shared" si="3"/>
         <v>4.6570057500054829E-2</v>
       </c>
     </row>
     <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="20">
-        <v>0</v>
-      </c>
-      <c r="C29" s="20">
+      <c r="B29" s="30">
+        <v>0</v>
+      </c>
+      <c r="C29" s="26">
         <v>2144</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="19">
         <f t="shared" si="2"/>
         <v>1.9654758303310323E-2</v>
       </c>
-      <c r="F29" s="23">
+      <c r="F29" s="20">
         <f t="shared" si="3"/>
         <v>1.9654758303310323E-2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" s="30">
         <v>422</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="26">
         <v>4151</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="19">
         <f t="shared" si="2"/>
         <v>8.3465189873417722E-2</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E30" s="19">
         <f t="shared" si="2"/>
         <v>3.8053592218769194E-2</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="20">
         <f t="shared" si="3"/>
         <v>-4.5411597654648528E-2</v>
       </c>
     </row>
     <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="20">
-        <v>0</v>
-      </c>
-      <c r="C31" s="20">
+      <c r="B31" s="30">
+        <v>0</v>
+      </c>
+      <c r="C31" s="26">
         <v>5721</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E31" s="19">
         <f t="shared" si="2"/>
         <v>5.2446302356920875E-2</v>
       </c>
-      <c r="F31" s="23">
+      <c r="F31" s="20">
         <f t="shared" si="3"/>
         <v>5.2446302356920875E-2</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="20">
+      <c r="B32" s="30">
         <v>608</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="26">
         <v>6886</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32" s="19">
         <f t="shared" si="2"/>
         <v>0.12025316455696203</v>
       </c>
-      <c r="E32" s="22">
+      <c r="E32" s="19">
         <f t="shared" si="2"/>
         <v>6.3126243319307315E-2</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="20">
         <f t="shared" si="3"/>
         <v>-5.7126921237654713E-2</v>
       </c>
     </row>
     <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="20">
-        <v>0</v>
-      </c>
-      <c r="C33" s="20">
+      <c r="B33" s="30">
+        <v>0</v>
+      </c>
+      <c r="C33" s="26">
         <v>809</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33" s="19">
         <f t="shared" si="2"/>
         <v>7.4163710202322999E-3</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="20">
         <f t="shared" si="3"/>
         <v>7.4163710202322999E-3</v>
       </c>
     </row>
     <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="20">
-        <v>0</v>
-      </c>
-      <c r="C34" s="20">
+      <c r="B34" s="30">
+        <v>0</v>
+      </c>
+      <c r="C34" s="26">
         <v>4124</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E34" s="22">
+      <c r="E34" s="19">
         <f t="shared" si="2"/>
         <v>3.7806074273718175E-2</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="20">
         <f t="shared" si="3"/>
         <v>3.7806074273718175E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="30">
         <v>8</v>
       </c>
-      <c r="C35" s="20">
+      <c r="C35" s="26">
         <v>6568</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="19">
         <f t="shared" si="2"/>
         <v>1.5822784810126582E-3</v>
       </c>
-      <c r="E35" s="22">
+      <c r="E35" s="19">
         <f t="shared" si="2"/>
         <v>6.0211031966484238E-2</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="20">
         <f t="shared" ref="F35:F47" si="4">E35-D35</f>
         <v>5.8628753485471578E-2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="20">
+      <c r="B36" s="30">
         <v>118</v>
       </c>
-      <c r="C36" s="20">
+      <c r="C36" s="26">
         <v>2394</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="19">
         <f t="shared" si="2"/>
         <v>2.3338607594936708E-2</v>
       </c>
-      <c r="E36" s="22">
+      <c r="E36" s="19">
         <f t="shared" si="2"/>
         <v>2.1946591127856768E-2</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="20">
         <f t="shared" si="4"/>
         <v>-1.3920164670799401E-3</v>
       </c>
     </row>
     <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="20">
-        <v>0</v>
-      </c>
-      <c r="C37" s="20">
+      <c r="B37" s="30">
+        <v>0</v>
+      </c>
+      <c r="C37" s="26">
         <v>4303</v>
       </c>
-      <c r="D37" s="22">
+      <c r="D37" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E37" s="22">
+      <c r="E37" s="19">
         <f t="shared" si="2"/>
         <v>3.9447026576093433E-2</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="20">
         <f t="shared" si="4"/>
         <v>3.9447026576093433E-2</v>
       </c>
     </row>
     <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="20">
-        <v>0</v>
-      </c>
-      <c r="C38" s="20">
+      <c r="B38" s="30">
+        <v>0</v>
+      </c>
+      <c r="C38" s="26">
         <v>1345</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D38" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E38" s="22">
+      <c r="E38" s="19">
         <f t="shared" si="2"/>
         <v>1.2330060596059881E-2</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="20">
         <f t="shared" si="4"/>
         <v>1.2330060596059881E-2</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="20">
+      <c r="B39" s="30">
         <v>2330</v>
       </c>
-      <c r="C39" s="20">
+      <c r="C39" s="26">
         <v>1174</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D39" s="19">
         <f t="shared" si="2"/>
         <v>0.46083860759493672</v>
       </c>
-      <c r="E39" s="22">
+      <c r="E39" s="19">
         <f t="shared" si="2"/>
         <v>1.0762446944070112E-2</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F39" s="20">
         <f t="shared" si="4"/>
         <v>-0.45007616065086659</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="20">
+      <c r="B40" s="30">
         <v>58</v>
       </c>
-      <c r="C40" s="20">
+      <c r="C40" s="26">
         <v>12479</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="19">
         <f t="shared" si="2"/>
         <v>1.1471518987341773E-2</v>
       </c>
-      <c r="E40" s="22">
+      <c r="E40" s="19">
         <f t="shared" si="2"/>
         <v>0.11439912727006041</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="20">
         <f t="shared" si="4"/>
         <v>0.10292760828271863</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="14" t="s">
+    <row r="41" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="20">
+      <c r="B41" s="30">
         <v>360</v>
       </c>
-      <c r="C41" s="20">
+      <c r="C41" s="26">
         <v>13832</v>
       </c>
-      <c r="D41" s="22">
+      <c r="D41" s="19">
         <f t="shared" si="2"/>
         <v>7.1202531645569625E-2</v>
       </c>
-      <c r="E41" s="22">
+      <c r="E41" s="19">
         <f t="shared" si="2"/>
         <v>0.12680252651650578</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F41" s="20">
         <f t="shared" si="4"/>
         <v>5.5599994870936156E-2</v>
       </c>
     </row>
     <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="20">
-        <v>0</v>
-      </c>
-      <c r="C42" s="20">
+      <c r="B42" s="30">
+        <v>0</v>
+      </c>
+      <c r="C42" s="26">
         <v>2427</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D42" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E42" s="22">
+      <c r="E42" s="19">
         <f t="shared" si="2"/>
         <v>2.22491130606969E-2</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F42" s="20">
         <f t="shared" si="4"/>
         <v>2.22491130606969E-2</v>
       </c>
     </row>
     <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="20">
-        <v>0</v>
-      </c>
-      <c r="C43" s="20">
+      <c r="B43" s="30">
+        <v>0</v>
+      </c>
+      <c r="C43" s="26">
         <v>7472</v>
       </c>
-      <c r="D43" s="22">
+      <c r="D43" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E43" s="22">
+      <c r="E43" s="19">
         <f t="shared" si="2"/>
         <v>6.8498299460044182E-2</v>
       </c>
-      <c r="F43" s="23">
+      <c r="F43" s="20">
         <f t="shared" si="4"/>
         <v>6.8498299460044182E-2</v>
       </c>
     </row>
     <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="20">
-        <v>0</v>
-      </c>
-      <c r="C44" s="20">
+      <c r="B44" s="30">
+        <v>0</v>
+      </c>
+      <c r="C44" s="26">
         <v>2728</v>
       </c>
-      <c r="D44" s="22">
+      <c r="D44" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E44" s="22">
+      <c r="E44" s="19">
         <f t="shared" si="2"/>
         <v>2.5008479781450821E-2</v>
       </c>
-      <c r="F44" s="23">
+      <c r="F44" s="20">
         <f t="shared" si="4"/>
         <v>2.5008479781450821E-2</v>
       </c>
     </row>
     <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="20">
-        <v>0</v>
-      </c>
-      <c r="C45" s="20">
+      <c r="B45" s="30">
+        <v>0</v>
+      </c>
+      <c r="C45" s="26">
         <v>9727</v>
       </c>
-      <c r="D45" s="22">
+      <c r="D45" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E45" s="22">
+      <c r="E45" s="19">
         <f t="shared" si="2"/>
         <v>8.9170631537453138E-2</v>
       </c>
-      <c r="F45" s="23">
+      <c r="F45" s="20">
         <f t="shared" si="4"/>
         <v>8.9170631537453138E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="14" t="s">
+    <row r="46" spans="1:6" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="20">
-        <v>0</v>
-      </c>
-      <c r="C46" s="20">
+      <c r="B46" s="30">
+        <v>0</v>
+      </c>
+      <c r="C46" s="26">
         <v>6955</v>
       </c>
-      <c r="D46" s="22">
+      <c r="D46" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E46" s="22">
+      <c r="E46" s="19">
         <f t="shared" si="2"/>
         <v>6.3758789178882141E-2</v>
       </c>
-      <c r="F46" s="23">
+      <c r="F46" s="20">
         <f t="shared" si="4"/>
         <v>6.3758789178882141E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="14" t="s">
+    <row r="47" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="20">
+      <c r="B47" s="31">
         <v>5056</v>
       </c>
-      <c r="C47" s="20">
+      <c r="C47" s="27">
         <v>109083</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="2">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="2">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="19"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="17"/>
     </row>
     <row r="59" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I59" s="3"/>
@@ -4644,10 +4808,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB8A44F-2AE7-4ADF-8B47-6F1BA901266B}">
-  <dimension ref="A1:L111"/>
+  <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L111"/>
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8883,7 +9047,18 @@
         <v>57.8611111111111</v>
       </c>
     </row>
+    <row r="113" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C113">
+        <f>SUM(C2:C90)</f>
+        <v>25745</v>
+      </c>
+      <c r="G113">
+        <f>SUM(G2:G90)</f>
+        <v>416661</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:L111" xr:uid="{DAB8A44F-2AE7-4ADF-8B47-6F1BA901266B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>